<commit_message>
Perfil Usuario css V4 y erratas
</commit_message>
<xml_diff>
--- a/Doc/SprintPlan18.xlsx
+++ b/Doc/SprintPlan18.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27624"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programacion\eclipse-workspace-tfg\proyectoGDV\Doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Álvaro\eclipse-workbench_TFG\proyectoGDV\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D6B3A981-5B45-464E-A8EA-28BC46E53D8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,9 +37,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
   <si>
-    <t>Sprint Plan 16 - GDV</t>
-  </si>
-  <si>
     <t>Actividades</t>
   </si>
   <si>
@@ -99,13 +95,16 @@
   </si>
   <si>
     <t>Documentación</t>
+  </si>
+  <si>
+    <t>Sprint Plan 18 - GDV</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -202,27 +201,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -502,124 +501,124 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D5:O26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9:L9"/>
+      <selection activeCell="D5" sqref="D5:O5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="6" max="6" width="28.85546875" customWidth="1"/>
-    <col min="12" max="12" width="80.85546875" customWidth="1"/>
+    <col min="6" max="6" width="28.88671875" customWidth="1"/>
+    <col min="12" max="12" width="80.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="4:15" ht="63.75" customHeight="1">
-      <c r="D5" s="5" t="s">
+    <row r="5" spans="4:15" ht="63.75" customHeight="1" x14ac:dyDescent="0.95">
+      <c r="D5" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9"/>
+      <c r="M5" s="9"/>
+      <c r="N5" s="9"/>
+      <c r="O5" s="9"/>
+    </row>
+    <row r="6" spans="4:15" ht="17.399999999999999" x14ac:dyDescent="0.45">
+      <c r="D6" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="5"/>
-      <c r="L5" s="5"/>
-      <c r="M5" s="5"/>
-      <c r="N5" s="5"/>
-      <c r="O5" s="5"/>
-    </row>
-    <row r="6" spans="4:15" ht="18.75">
-      <c r="D6" s="8" t="s">
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="10" t="s">
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="H6" s="9"/>
-      <c r="I6" s="9"/>
-      <c r="J6" s="10" t="s">
+      <c r="K6" s="11"/>
+      <c r="L6" s="11"/>
+      <c r="M6" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="K6" s="9"/>
-      <c r="L6" s="9"/>
-      <c r="M6" s="10" t="s">
+      <c r="N6" s="11"/>
+      <c r="O6" s="11"/>
+    </row>
+    <row r="7" spans="4:15" x14ac:dyDescent="0.3">
+      <c r="D7" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="N6" s="9"/>
-      <c r="O6" s="9"/>
-    </row>
-    <row r="7" spans="4:15">
-      <c r="D7" s="6" t="s">
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="12"/>
+      <c r="K7" s="12"/>
+      <c r="L7" s="12"/>
+      <c r="M7" s="12"/>
+      <c r="N7" s="12"/>
+      <c r="O7" s="12"/>
+    </row>
+    <row r="8" spans="4:15" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D8" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="6"/>
-      <c r="L7" s="6"/>
-      <c r="M7" s="6"/>
-      <c r="N7" s="6"/>
-      <c r="O7" s="6"/>
-    </row>
-    <row r="8" spans="4:15" ht="36" customHeight="1">
-      <c r="D8" s="7" t="s">
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="3" t="s">
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3" t="s">
+      <c r="K8" s="6"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3"/>
-      <c r="M8" s="3" t="s">
+      <c r="N8" s="6"/>
+      <c r="O8" s="6"/>
+    </row>
+    <row r="9" spans="4:15" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D9" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="N8" s="3"/>
-      <c r="O8" s="3"/>
-    </row>
-    <row r="9" spans="4:15" ht="33" customHeight="1">
-      <c r="D9" s="11" t="s">
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
-      <c r="J9" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="K9" s="3"/>
-      <c r="L9" s="3"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="6"/>
       <c r="M9" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="N9" s="4"/>
-      <c r="O9" s="4"/>
-    </row>
-    <row r="10" spans="4:15">
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="11"/>
+        <v>8</v>
+      </c>
+      <c r="N9" s="7"/>
+      <c r="O9" s="7"/>
+    </row>
+    <row r="10" spans="4:15" x14ac:dyDescent="0.3">
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
@@ -627,13 +626,13 @@
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
     </row>
-    <row r="11" spans="4:15">
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="11"/>
-      <c r="I11" s="11"/>
+    <row r="11" spans="4:15" x14ac:dyDescent="0.3">
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
@@ -641,73 +640,73 @@
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
     </row>
-    <row r="12" spans="4:15">
-      <c r="D12" s="12" t="s">
+    <row r="12" spans="4:15" x14ac:dyDescent="0.3">
+      <c r="D12" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="4"/>
+      <c r="M12" s="4"/>
+      <c r="N12" s="4"/>
+      <c r="O12" s="4"/>
+    </row>
+    <row r="13" spans="4:15" x14ac:dyDescent="0.3">
+      <c r="D13" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
-      <c r="H12" s="13"/>
-      <c r="I12" s="13"/>
-      <c r="J12" s="13"/>
-      <c r="K12" s="13"/>
-      <c r="L12" s="13"/>
-      <c r="M12" s="13"/>
-      <c r="N12" s="13"/>
-      <c r="O12" s="13"/>
-    </row>
-    <row r="13" spans="4:15">
-      <c r="D13" s="11" t="s">
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="H13" s="11"/>
-      <c r="I13" s="11"/>
-      <c r="J13" s="2" t="s">
-        <v>14</v>
       </c>
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
       <c r="M13" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="N13" s="2"/>
       <c r="O13" s="2"/>
     </row>
-    <row r="14" spans="4:15">
-      <c r="D14" s="11" t="s">
+    <row r="14" spans="4:15" x14ac:dyDescent="0.3">
+      <c r="D14" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="H14" s="11"/>
-      <c r="I14" s="11"/>
-      <c r="J14" s="2" t="s">
-        <v>17</v>
       </c>
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
       <c r="M14" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="N14" s="2"/>
       <c r="O14" s="2"/>
     </row>
-    <row r="15" spans="4:15">
-      <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="11"/>
-      <c r="I15" s="11"/>
+    <row r="15" spans="4:15" x14ac:dyDescent="0.3">
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
@@ -715,7 +714,7 @@
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
     </row>
-    <row r="16" spans="4:15">
+    <row r="16" spans="4:15" x14ac:dyDescent="0.3">
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
@@ -729,26 +728,26 @@
       <c r="N16" s="1"/>
       <c r="O16" s="1"/>
     </row>
-    <row r="17" spans="4:15">
-      <c r="D17" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
-      <c r="H17" s="13"/>
-      <c r="I17" s="13"/>
-      <c r="J17" s="13"/>
-      <c r="K17" s="13"/>
-      <c r="L17" s="13"/>
-      <c r="M17" s="13"/>
-      <c r="N17" s="13"/>
-      <c r="O17" s="13"/>
-    </row>
-    <row r="18" spans="4:15">
-      <c r="D18" s="11"/>
-      <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
+    <row r="17" spans="4:15" x14ac:dyDescent="0.3">
+      <c r="D17" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="4"/>
+      <c r="K17" s="4"/>
+      <c r="L17" s="4"/>
+      <c r="M17" s="4"/>
+      <c r="N17" s="4"/>
+      <c r="O17" s="4"/>
+    </row>
+    <row r="18" spans="4:15" x14ac:dyDescent="0.3">
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
@@ -759,10 +758,10 @@
       <c r="N18" s="2"/>
       <c r="O18" s="2"/>
     </row>
-    <row r="19" spans="4:15">
-      <c r="D19" s="11"/>
-      <c r="E19" s="11"/>
-      <c r="F19" s="11"/>
+    <row r="19" spans="4:15" x14ac:dyDescent="0.3">
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
@@ -773,10 +772,10 @@
       <c r="N19" s="2"/>
       <c r="O19" s="2"/>
     </row>
-    <row r="20" spans="4:15">
-      <c r="D20" s="11"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="11"/>
+    <row r="20" spans="4:15" x14ac:dyDescent="0.3">
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
@@ -787,10 +786,10 @@
       <c r="N20" s="1"/>
       <c r="O20" s="1"/>
     </row>
-    <row r="21" spans="4:15">
-      <c r="D21" s="11"/>
-      <c r="E21" s="11"/>
-      <c r="F21" s="11"/>
+    <row r="21" spans="4:15" x14ac:dyDescent="0.3">
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
@@ -801,26 +800,26 @@
       <c r="N21" s="1"/>
       <c r="O21" s="1"/>
     </row>
-    <row r="22" spans="4:15">
-      <c r="D22" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="13"/>
-      <c r="H22" s="13"/>
-      <c r="I22" s="13"/>
-      <c r="J22" s="13"/>
-      <c r="K22" s="13"/>
-      <c r="L22" s="13"/>
-      <c r="M22" s="13"/>
-      <c r="N22" s="13"/>
-      <c r="O22" s="13"/>
-    </row>
-    <row r="23" spans="4:15">
-      <c r="D23" s="11"/>
-      <c r="E23" s="11"/>
-      <c r="F23" s="11"/>
+    <row r="22" spans="4:15" x14ac:dyDescent="0.3">
+      <c r="D22" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="4"/>
+      <c r="I22" s="4"/>
+      <c r="J22" s="4"/>
+      <c r="K22" s="4"/>
+      <c r="L22" s="4"/>
+      <c r="M22" s="4"/>
+      <c r="N22" s="4"/>
+      <c r="O22" s="4"/>
+    </row>
+    <row r="23" spans="4:15" x14ac:dyDescent="0.3">
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
@@ -831,10 +830,10 @@
       <c r="N23" s="2"/>
       <c r="O23" s="2"/>
     </row>
-    <row r="24" spans="4:15">
-      <c r="D24" s="11"/>
-      <c r="E24" s="11"/>
-      <c r="F24" s="11"/>
+    <row r="24" spans="4:15" x14ac:dyDescent="0.3">
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
@@ -845,10 +844,10 @@
       <c r="N24" s="2"/>
       <c r="O24" s="2"/>
     </row>
-    <row r="25" spans="4:15">
-      <c r="D25" s="11"/>
-      <c r="E25" s="11"/>
-      <c r="F25" s="11"/>
+    <row r="25" spans="4:15" x14ac:dyDescent="0.3">
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
@@ -859,10 +858,10 @@
       <c r="N25" s="1"/>
       <c r="O25" s="1"/>
     </row>
-    <row r="26" spans="4:15">
-      <c r="D26" s="11"/>
-      <c r="E26" s="11"/>
-      <c r="F26" s="11"/>
+    <row r="26" spans="4:15" x14ac:dyDescent="0.3">
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
@@ -887,6 +886,10 @@
     <mergeCell ref="D9:F9"/>
     <mergeCell ref="D10:F10"/>
     <mergeCell ref="D11:F11"/>
+    <mergeCell ref="J8:L8"/>
+    <mergeCell ref="J9:L9"/>
+    <mergeCell ref="J10:L10"/>
+    <mergeCell ref="J11:L11"/>
     <mergeCell ref="D24:F24"/>
     <mergeCell ref="D14:F14"/>
     <mergeCell ref="D15:F15"/>
@@ -913,10 +916,6 @@
     <mergeCell ref="G21:I21"/>
     <mergeCell ref="G23:I23"/>
     <mergeCell ref="G24:I24"/>
-    <mergeCell ref="J8:L8"/>
-    <mergeCell ref="J9:L9"/>
-    <mergeCell ref="J10:L10"/>
-    <mergeCell ref="J11:L11"/>
     <mergeCell ref="J13:L13"/>
     <mergeCell ref="M14:O14"/>
     <mergeCell ref="M15:O15"/>

</xml_diff>